<commit_message>
operaciones aritmeticas y compilacion
</commit_message>
<xml_diff>
--- a/archivos/comandos.xlsx
+++ b/archivos/comandos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emily\Desktop\CE4301-Proyecto1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emily\Desktop\CE4301-Proyecto1\archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2427EAC3-17AD-4703-A09F-EFA458D78466}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92228D7A-E06E-4195-BAF2-01FD767176E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18375" yWindow="2805" windowWidth="17280" windowHeight="8970" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20520" yWindow="780" windowWidth="20640" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="148">
   <si>
     <t>Escritura y lectura *(tenemos que hablar de estos metodos)</t>
   </si>
@@ -447,6 +447,30 @@
   </si>
   <si>
     <t>OOO111</t>
+  </si>
+  <si>
+    <t>div R1,R1,#2</t>
+  </si>
+  <si>
+    <t>mul R1,R1,#2</t>
+  </si>
+  <si>
+    <t>and R1,R1,R2</t>
+  </si>
+  <si>
+    <t>or R1,R1,R2</t>
+  </si>
+  <si>
+    <t>OOO1OOOOO1OO1OOOOOOOOOOOOOOOOO11</t>
+  </si>
+  <si>
+    <t>OOO1O1OOOO1OO1OOOOOOOOOOOOOOOOO11</t>
+  </si>
+  <si>
+    <t>OOO11OOOO1OO1O1OOOOOOOOOOOOOOOOO</t>
+  </si>
+  <si>
+    <t>OOO111OOO1OO1O1OOOOOOOOOOOOOOOOO</t>
   </si>
 </sst>
 </file>
@@ -684,6 +708,15 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -691,19 +724,10 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2095,7 +2119,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:B29"/>
+      <selection activeCell="A2" sqref="A2:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
@@ -2106,10 +2130,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="22"/>
+      <c r="B1" s="25"/>
     </row>
     <row r="2" spans="1:6" ht="15.6">
       <c r="A2" s="7" t="s">
@@ -2218,10 +2242,10 @@
       <c r="B14" s="16"/>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="22"/>
+      <c r="B15" s="25"/>
     </row>
     <row r="16" spans="1:6" ht="15.6">
       <c r="A16" s="7" t="s">
@@ -2316,10 +2340,10 @@
       <c r="B27" s="19"/>
     </row>
     <row r="28" spans="1:2" ht="15" customHeight="1">
-      <c r="A28" s="23" t="s">
+      <c r="A28" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="B28" s="22"/>
+      <c r="B28" s="25"/>
     </row>
     <row r="29" spans="1:2" ht="15.6">
       <c r="A29" s="11" t="s">
@@ -2389,17 +2413,17 @@
   <dimension ref="A2:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="11.296875" style="26" customWidth="1"/>
-    <col min="2" max="2" width="12.69921875" style="26" customWidth="1"/>
-    <col min="3" max="3" width="48.296875" style="26" customWidth="1"/>
-    <col min="4" max="5" width="14.69921875" style="26" customWidth="1"/>
-    <col min="6" max="6" width="10.8984375" style="26" customWidth="1"/>
-    <col min="7" max="16384" width="8.796875" style="26"/>
+    <col min="1" max="1" width="11.296875" style="22" customWidth="1"/>
+    <col min="2" max="2" width="12.69921875" style="22" customWidth="1"/>
+    <col min="3" max="3" width="48.296875" style="22" customWidth="1"/>
+    <col min="4" max="5" width="14.69921875" style="22" customWidth="1"/>
+    <col min="6" max="6" width="10.8984375" style="22" customWidth="1"/>
+    <col min="7" max="16384" width="8.796875" style="22"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:12">
@@ -2419,72 +2443,72 @@
       <c r="K2" s="27"/>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="F3" s="26">
+      <c r="F3" s="22">
         <v>31</v>
       </c>
-      <c r="K3" s="26">
+      <c r="K3" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="G4" s="25" t="s">
+      <c r="G4" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="H4" s="25" t="s">
+      <c r="H4" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="I4" s="25" t="s">
+      <c r="I4" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="J4" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="K4" s="25" t="s">
+      <c r="K4" s="21" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="24"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="25" t="s">
+      <c r="A5" s="28"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="29" t="s">
@@ -2493,142 +2517,158 @@
       <c r="B6" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="30"/>
       <c r="B7" s="30"/>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="G7" s="26" t="s">
+      <c r="G7" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="H7" s="26" t="s">
+      <c r="H7" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="I7" s="26" t="s">
+      <c r="I7" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="J7" s="26" t="s">
+      <c r="J7" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="K7" s="26" t="s">
+      <c r="K7" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="L7" s="26" t="s">
+      <c r="L7" s="22" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="F8" s="26" t="s">
+      <c r="F8" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="G8" s="26" t="s">
+      <c r="G8" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="H8" s="26" t="s">
+      <c r="H8" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="I8" s="26" t="s">
+      <c r="I8" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="J8" s="26" t="s">
+      <c r="J8" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="K8" s="26" t="s">
+      <c r="K8" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="L8" s="26" t="s">
+      <c r="L8" s="22" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="F9" s="26">
+      <c r="C9" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="F9" s="22">
         <v>6</v>
       </c>
-      <c r="G9" s="26">
+      <c r="G9" s="22">
         <v>4</v>
       </c>
-      <c r="H9" s="26">
+      <c r="H9" s="22">
         <v>3</v>
       </c>
-      <c r="I9" s="26">
+      <c r="I9" s="22">
         <v>3</v>
       </c>
-      <c r="J9" s="26">
+      <c r="J9" s="22">
         <v>8</v>
       </c>
-      <c r="K9" s="26">
+      <c r="K9" s="22">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
+      <c r="C10" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
+      <c r="C11" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
+      <c r="C12" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>143</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
integracion de ope aritmetico/logicas y tb
</commit_message>
<xml_diff>
--- a/archivos/comandos.xlsx
+++ b/archivos/comandos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emily\Desktop\CE4301-Proyecto1\archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92228D7A-E06E-4195-BAF2-01FD767176E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021A9D6F-69A0-49A3-ACFD-D9C85A433C65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20520" yWindow="780" windowWidth="20640" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20520" yWindow="780" windowWidth="20640" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="154">
   <si>
     <t>Escritura y lectura *(tenemos que hablar de estos metodos)</t>
   </si>
@@ -140,9 +140,6 @@
     <t>Sin desbordamiento, la suma de &amp;R2+&amp;R3 se guarda en &amp;R1</t>
   </si>
   <si>
-    <t xml:space="preserve">SUMAI &amp;R1, &amp;R2, #(16 bits) </t>
-  </si>
-  <si>
     <t>Sin desbordamiento, la suma de R2+# se guarda en &amp;R1</t>
   </si>
   <si>
@@ -152,9 +149,6 @@
     <t>Sin desbordamiento, la resta de &amp;R2-&amp;R3 se guarda en &amp;R1</t>
   </si>
   <si>
-    <t>RESTAI &amp;R1, &amp;R2, #(16 bits)</t>
-  </si>
-  <si>
     <t>Sin desbordamiento, la resta de R2-# se guarda en &amp;R1</t>
   </si>
   <si>
@@ -164,15 +158,9 @@
     <t>Sin desbordamiento, la division de &amp;R2/# se guarda en &amp;R1</t>
   </si>
   <si>
-    <t xml:space="preserve">RESUDIV $R1 </t>
-  </si>
-  <si>
     <t>Mueve el valor dentro del registro resultado a &amp;R1, Este es el resultado de la instruccion DIVISION</t>
   </si>
   <si>
-    <t xml:space="preserve">RESIDIV $R1 </t>
-  </si>
-  <si>
     <t>MULT &amp;R1, &amp;R2, &amp;R3</t>
   </si>
   <si>
@@ -197,12 +185,6 @@
     <t>Realiza la opracion binarIa or de R1 v R2 se guarda en R1</t>
   </si>
   <si>
-    <t xml:space="preserve">addi $t1,$t2, 4 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Addition immediate with overflow : set $t1 to ($t2 plus signed 16-bit immediate) ejemplo $t4=0x0111102333         adii $t4,$t4,4 aumento 4 en memoria </t>
-  </si>
-  <si>
     <t>Control de flujo</t>
   </si>
   <si>
@@ -305,12 +287,6 @@
     <t>Escribe el valor contenido en R1 en la posicion de memoria por R2</t>
   </si>
   <si>
-    <t>LA</t>
-  </si>
-  <si>
-    <t>Revisar</t>
-  </si>
-  <si>
     <t>Nota: Hablar de las operaciones</t>
   </si>
   <si>
@@ -335,15 +311,9 @@
     <t>oooooooo</t>
   </si>
   <si>
-    <t>ooo1</t>
-  </si>
-  <si>
     <t>ooooo1o1</t>
   </si>
   <si>
-    <t>Resultado</t>
-  </si>
-  <si>
     <t>suma R1, R1+ R2</t>
   </si>
   <si>
@@ -471,13 +441,77 @@
   </si>
   <si>
     <t>OOO111OOO1OO1O1OOOOOOOOOOOOOOOOO</t>
+  </si>
+  <si>
+    <t>LDR</t>
+  </si>
+  <si>
+    <t>OO1OOO</t>
+  </si>
+  <si>
+    <t>OO1OO1</t>
+  </si>
+  <si>
+    <t>OO1OO1O</t>
+  </si>
+  <si>
+    <t>str R1,#4</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>o</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>oo1</t>
+    </r>
+  </si>
+  <si>
+    <t>STRMD</t>
+  </si>
+  <si>
+    <t>STRMI</t>
+  </si>
+  <si>
+    <t>OO1OOOOOOOOOO1OOOOOOOOOOOOOOO1OO</t>
+  </si>
+  <si>
+    <t>Destino</t>
+  </si>
+  <si>
+    <t>str R1,[R2]</t>
+  </si>
+  <si>
+    <t>ldr R1,[R2]</t>
+  </si>
+  <si>
+    <t>strim R1</t>
+  </si>
+  <si>
+    <t>0 - FF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUMA &amp;R1, &amp;R2, #(16 bits) </t>
+  </si>
+  <si>
+    <t>RESTA &amp;R1, &amp;R2, #(16 bits)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -537,6 +571,18 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -559,12 +605,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF00FF00"/>
         <bgColor rgb="FF00FF00"/>
       </patternFill>
@@ -581,8 +621,14 @@
         <bgColor rgb="FFFF00FF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -668,11 +714,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -696,18 +751,13 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -717,11 +767,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -745,6 +801,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2118,8 +2188,8 @@
   </sheetPr>
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A12"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
@@ -2130,10 +2200,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="25"/>
+      <c r="B1" s="24"/>
     </row>
     <row r="2" spans="1:6" ht="15.6">
       <c r="A2" s="7" t="s">
@@ -2145,257 +2215,245 @@
     </row>
     <row r="3" spans="1:6" ht="15.6">
       <c r="A3" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>37</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.6">
       <c r="A4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>39</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>40</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:6" ht="15.6">
       <c r="A5" s="7" t="s">
-        <v>41</v>
+        <v>153</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.6">
       <c r="A6" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.6">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.6">
-      <c r="A7" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="8" spans="1:6" ht="15.6">
-      <c r="A8" s="10" t="s">
-        <v>47</v>
-      </c>
+      <c r="A8" s="10"/>
       <c r="B8" s="8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.6">
       <c r="A9" s="7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.6">
       <c r="A10" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.6">
       <c r="A11" s="11" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:6" ht="15.6">
       <c r="A12" s="11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.6">
-      <c r="A13" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
+      <c r="A13" s="36"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
     </row>
     <row r="14" spans="1:6" ht="15.6">
-      <c r="A14" s="15"/>
-      <c r="B14" s="16"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="13"/>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1">
-      <c r="A15" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="B15" s="25"/>
+      <c r="A15" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="24"/>
     </row>
     <row r="16" spans="1:6" ht="15.6">
       <c r="A16" s="7" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.6">
       <c r="A17" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>62</v>
+        <v>55</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.6">
       <c r="A18" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>64</v>
+        <v>57</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15" customHeight="1">
       <c r="A19" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>66</v>
+        <v>59</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15.6">
       <c r="A20" s="11" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15" customHeight="1">
       <c r="A21" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>70</v>
+        <v>63</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15" customHeight="1">
       <c r="A22" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>72</v>
+        <v>65</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15" customHeight="1">
       <c r="A23" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>74</v>
+        <v>67</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.6">
       <c r="A24" s="11" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15.6">
       <c r="A25" s="11" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.6">
       <c r="A26" s="10" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.6">
-      <c r="A27" s="18"/>
-      <c r="B27" s="19"/>
+      <c r="A27" s="15"/>
+      <c r="B27" s="16"/>
     </row>
     <row r="28" spans="1:2" ht="15" customHeight="1">
-      <c r="A28" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="B28" s="25"/>
+      <c r="A28" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="B28" s="24"/>
     </row>
     <row r="29" spans="1:2" ht="15.6">
       <c r="A29" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="B29" s="17" t="s">
-        <v>83</v>
+        <v>76</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.6">
       <c r="A30" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B30" s="17" t="s">
-        <v>85</v>
+        <v>78</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.6">
       <c r="A31" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="B31" s="17" t="s">
-        <v>87</v>
+        <v>80</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.6">
       <c r="A32" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="B32" s="17" t="s">
-        <v>89</v>
+        <v>82</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.6">
       <c r="A33" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="B33" s="17" t="s">
-        <v>91</v>
+        <v>84</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="14.4">
-      <c r="A34" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="B34" s="13" t="s">
-        <v>93</v>
-      </c>
+      <c r="A34" s="37"/>
+      <c r="B34" s="37"/>
     </row>
     <row r="36" spans="1:2" ht="15.6">
-      <c r="B36" s="20" t="s">
-        <v>94</v>
+      <c r="B36" s="17" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -2410,268 +2468,323 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{935F8D7C-FEC4-4F7D-8C36-4AF6CEC33DFE}">
-  <dimension ref="A2:L12"/>
+  <dimension ref="A2:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="11.296875" style="22" customWidth="1"/>
-    <col min="2" max="2" width="12.69921875" style="22" customWidth="1"/>
-    <col min="3" max="3" width="48.296875" style="22" customWidth="1"/>
-    <col min="4" max="5" width="14.69921875" style="22" customWidth="1"/>
-    <col min="6" max="6" width="10.8984375" style="22" customWidth="1"/>
-    <col min="7" max="16384" width="8.796875" style="22"/>
+    <col min="1" max="1" width="11.296875" style="19" customWidth="1"/>
+    <col min="2" max="2" width="12.69921875" style="19" customWidth="1"/>
+    <col min="3" max="3" width="48.296875" style="19" customWidth="1"/>
+    <col min="4" max="5" width="14.69921875" style="19" customWidth="1"/>
+    <col min="6" max="6" width="10.8984375" style="19" customWidth="1"/>
+    <col min="7" max="11" width="8.796875" style="19"/>
+    <col min="12" max="13" width="16.69921875" style="19" customWidth="1"/>
+    <col min="14" max="16384" width="8.796875" style="19"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:12">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="32"/>
+      <c r="F2" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="F3" s="19">
+        <v>31</v>
+      </c>
+      <c r="K3" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="J4" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="K4" s="18" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="29"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="H7" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="J7" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="K7" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="L7" s="19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="G8" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="I8" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="J8" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="K8" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="L8" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="F9" s="19">
+        <v>6</v>
+      </c>
+      <c r="G9" s="19">
+        <v>4</v>
+      </c>
+      <c r="H9" s="19">
+        <v>3</v>
+      </c>
+      <c r="I9" s="19">
+        <v>3</v>
+      </c>
+      <c r="J9" s="19">
+        <v>8</v>
+      </c>
+      <c r="K9" s="19">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="33"/>
-      <c r="F2" s="27" t="s">
-        <v>113</v>
-      </c>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>125</v>
-      </c>
-      <c r="F3" s="22">
-        <v>31</v>
-      </c>
-      <c r="K3" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" s="28" t="s">
-        <v>114</v>
-      </c>
-      <c r="B4" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="C4" s="21" t="s">
+      <c r="B12" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D12" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="D4" s="21" t="s">
-        <v>128</v>
-      </c>
-      <c r="F4" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="G4" s="21" t="s">
-        <v>104</v>
-      </c>
-      <c r="H4" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="I4" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="J4" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="K4" s="21" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="28"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="21" t="s">
-        <v>130</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>129</v>
-      </c>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="B6" s="29" t="s">
-        <v>116</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>134</v>
-      </c>
-      <c r="D6" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="30"/>
-      <c r="B7" s="30"/>
-      <c r="C7" s="21" t="s">
-        <v>135</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="F7" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="G7" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="H7" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="I7" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="J7" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="K7" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="L7" s="22" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>118</v>
-      </c>
-      <c r="C8" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="F8" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="G8" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="H8" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="I8" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="J8" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="K8" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="L8" s="22" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="C9" s="21" t="s">
+    </row>
+    <row r="13" spans="1:12" s="21" customFormat="1">
+      <c r="A13" s="34" t="s">
         <v>144</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="B13" s="35" t="s">
+        <v>139</v>
+      </c>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="33"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="B15" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="F9" s="22">
-        <v>6</v>
-      </c>
-      <c r="G9" s="22">
-        <v>4</v>
-      </c>
-      <c r="H9" s="22">
-        <v>3</v>
-      </c>
-      <c r="I9" s="22">
-        <v>3</v>
-      </c>
-      <c r="J9" s="22">
-        <v>8</v>
-      </c>
-      <c r="K9" s="22">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="C10" s="21" t="s">
+      <c r="C15" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="D10" s="21" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>138</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="D12" s="21" t="s">
-        <v>143</v>
+    </row>
+    <row r="17" spans="4:4">
+      <c r="D17" s="19" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4">
+      <c r="D18" s="19" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
     <mergeCell ref="F2:K2"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
@@ -2680,5 +2793,6 @@
     <mergeCell ref="A2:D2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modificaciones en el greenshit
</commit_message>
<xml_diff>
--- a/archivos/comandos.xlsx
+++ b/archivos/comandos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emily\Desktop\CE4301-Proyecto1\archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021A9D6F-69A0-49A3-ACFD-D9C85A433C65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98ABE9A7-F9F6-4496-A471-04352D243177}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20520" yWindow="780" windowWidth="20640" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20520" yWindow="780" windowWidth="20640" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="162">
   <si>
     <t>Escritura y lectura *(tenemos que hablar de estos metodos)</t>
   </si>
@@ -443,16 +443,10 @@
     <t>OOO111OOO1OO1O1OOOOOOOOOOOOOOOOO</t>
   </si>
   <si>
-    <t>LDR</t>
-  </si>
-  <si>
     <t>OO1OOO</t>
   </si>
   <si>
     <t>OO1OO1</t>
-  </si>
-  <si>
-    <t>OO1OO1O</t>
   </si>
   <si>
     <t>str R1,#4</t>
@@ -495,16 +489,46 @@
     <t>ldr R1,[R2]</t>
   </si>
   <si>
-    <t>strim R1</t>
-  </si>
-  <si>
-    <t>0 - FF</t>
-  </si>
-  <si>
     <t xml:space="preserve">SUMA &amp;R1, &amp;R2, #(16 bits) </t>
   </si>
   <si>
     <t>RESTA &amp;R1, &amp;R2, #(16 bits)</t>
+  </si>
+  <si>
+    <t>LDRMD</t>
+  </si>
+  <si>
+    <t>LDRMI</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>S #4</t>
+  </si>
+  <si>
+    <t>OO1O1O</t>
+  </si>
+  <si>
+    <t>OO1O11</t>
+  </si>
+  <si>
+    <t>OO11OO</t>
+  </si>
+  <si>
+    <t>SEQ R1,R2,#4</t>
+  </si>
+  <si>
+    <t>SEQ</t>
+  </si>
+  <si>
+    <t>OO11O1</t>
+  </si>
+  <si>
+    <t>OO11O1OOOOOO1O1OOOOOO1OOOOOOOOOO</t>
+  </si>
+  <si>
+    <t>OO11OOOOOOOOOOOOOOOOO1OOOOOOOOO</t>
   </si>
 </sst>
 </file>
@@ -727,7 +751,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -773,12 +797,26 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -801,20 +839,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2188,8 +2227,8 @@
   </sheetPr>
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
@@ -2200,10 +2239,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="24"/>
+      <c r="B1" s="27"/>
     </row>
     <row r="2" spans="1:6" ht="15.6">
       <c r="A2" s="7" t="s">
@@ -2215,7 +2254,7 @@
     </row>
     <row r="3" spans="1:6" ht="15.6">
       <c r="A3" s="7" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>37</v>
@@ -2232,7 +2271,7 @@
     </row>
     <row r="5" spans="1:6" ht="15.6">
       <c r="A5" s="7" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>40</v>
@@ -2292,22 +2331,22 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.6">
-      <c r="A13" s="36"/>
-      <c r="B13" s="37"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
+      <c r="A13" s="23"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
     </row>
     <row r="14" spans="1:6" ht="15.6">
       <c r="A14" s="12"/>
       <c r="B14" s="13"/>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B15" s="24"/>
+      <c r="B15" s="27"/>
     </row>
     <row r="16" spans="1:6" ht="15.6">
       <c r="A16" s="7" t="s">
@@ -2402,10 +2441,10 @@
       <c r="B27" s="16"/>
     </row>
     <row r="28" spans="1:2" ht="15" customHeight="1">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="B28" s="24"/>
+      <c r="B28" s="27"/>
     </row>
     <row r="29" spans="1:2" ht="15.6">
       <c r="A29" s="11" t="s">
@@ -2448,8 +2487,8 @@
       </c>
     </row>
     <row r="34" spans="1:2" ht="14.4">
-      <c r="A34" s="37"/>
-      <c r="B34" s="37"/>
+      <c r="A34" s="24"/>
+      <c r="B34" s="24"/>
     </row>
     <row r="36" spans="1:2" ht="15.6">
       <c r="B36" s="17" t="s">
@@ -2468,10 +2507,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{935F8D7C-FEC4-4F7D-8C36-4AF6CEC33DFE}">
-  <dimension ref="A2:L18"/>
+  <dimension ref="A2:L27"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2487,20 +2526,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="32"/>
-      <c r="F2" s="26" t="s">
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="38"/>
+      <c r="F2" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="18" t="s">
@@ -2523,10 +2562,10 @@
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="33" t="s">
         <v>104</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="33" t="s">
         <v>105</v>
       </c>
       <c r="C4" s="18" t="s">
@@ -2539,7 +2578,7 @@
         <v>87</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H4" s="18" t="s">
         <v>88</v>
@@ -2555,8 +2594,8 @@
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="27"/>
-      <c r="B5" s="27"/>
+      <c r="A5" s="33"/>
+      <c r="B5" s="33"/>
       <c r="C5" s="18" t="s">
         <v>120</v>
       </c>
@@ -2571,10 +2610,10 @@
       <c r="K5" s="20"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="34" t="s">
         <v>106</v>
       </c>
       <c r="C6" s="18" t="s">
@@ -2591,8 +2630,8 @@
       <c r="K6" s="20"/>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="29"/>
-      <c r="B7" s="29"/>
+      <c r="A7" s="35"/>
+      <c r="B7" s="35"/>
       <c r="C7" s="18" t="s">
         <v>125</v>
       </c>
@@ -2603,7 +2642,7 @@
         <v>92</v>
       </c>
       <c r="G7" s="22" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H7" s="19" t="s">
         <v>97</v>
@@ -2638,7 +2677,7 @@
         <v>92</v>
       </c>
       <c r="G8" s="22" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H8" s="19" t="s">
         <v>98</v>
@@ -2731,55 +2770,139 @@
       </c>
     </row>
     <row r="13" spans="1:12" s="21" customFormat="1">
-      <c r="A13" s="34" t="s">
-        <v>144</v>
-      </c>
-      <c r="B13" s="35" t="s">
-        <v>139</v>
+      <c r="A13" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>138</v>
       </c>
       <c r="C13" s="20"/>
       <c r="D13" s="20" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="33"/>
-      <c r="B14" s="26"/>
+      <c r="A14" s="30"/>
+      <c r="B14" s="32"/>
       <c r="C14" s="19" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>142</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="19" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
+        <v>147</v>
+      </c>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+    </row>
+    <row r="16" spans="1:12" ht="15.6">
       <c r="A16" s="22" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="17" spans="4:4">
-      <c r="D17" s="19" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="18" spans="4:4">
+        <v>143</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="E16" s="40"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="39"/>
+    </row>
+    <row r="17" spans="1:7" ht="15.6">
+      <c r="A17" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="E17" s="42"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="39"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.6">
+      <c r="A18" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>161</v>
+      </c>
       <c r="D18" s="19" t="s">
-        <v>151</v>
-      </c>
+        <v>153</v>
+      </c>
+      <c r="E18" s="42"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="39"/>
+    </row>
+    <row r="19" spans="1:7" ht="15.6">
+      <c r="A19" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="E19" s="44"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="39"/>
+    </row>
+    <row r="20" spans="1:7" ht="15.6">
+      <c r="E20" s="44"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="39"/>
+    </row>
+    <row r="21" spans="1:7" ht="15.6">
+      <c r="E21" s="44"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="39"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.6">
+      <c r="E22" s="44"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="39"/>
+    </row>
+    <row r="23" spans="1:7" ht="15.6">
+      <c r="E23" s="44"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="39"/>
+    </row>
+    <row r="24" spans="1:7" ht="15.6">
+      <c r="E24" s="44"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="39"/>
+    </row>
+    <row r="25" spans="1:7" ht="15.6">
+      <c r="E25" s="44"/>
+      <c r="F25" s="41"/>
+      <c r="G25" s="39"/>
+    </row>
+    <row r="26" spans="1:7" ht="15.6">
+      <c r="E26" s="42"/>
+      <c r="F26" s="45"/>
+      <c r="G26" s="39"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="E27" s="39"/>
+      <c r="F27" s="39"/>
+      <c r="G27" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
str y ldr para imagenes y datos
</commit_message>
<xml_diff>
--- a/archivos/comandos.xlsx
+++ b/archivos/comandos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emily\Desktop\CE4301-Proyecto1\archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98ABE9A7-F9F6-4496-A471-04352D243177}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89BF728A-390C-4AA5-B922-88FD6338C837}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20520" yWindow="780" windowWidth="20640" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -802,6 +802,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -839,21 +854,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2227,8 +2227,8 @@
   </sheetPr>
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
@@ -2239,10 +2239,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="27"/>
+      <c r="B1" s="34"/>
     </row>
     <row r="2" spans="1:6" ht="15.6">
       <c r="A2" s="7" t="s">
@@ -2343,10 +2343,10 @@
       <c r="B14" s="13"/>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="B15" s="27"/>
+      <c r="B15" s="34"/>
     </row>
     <row r="16" spans="1:6" ht="15.6">
       <c r="A16" s="7" t="s">
@@ -2441,10 +2441,10 @@
       <c r="B27" s="16"/>
     </row>
     <row r="28" spans="1:2" ht="15" customHeight="1">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="B28" s="27"/>
+      <c r="B28" s="34"/>
     </row>
     <row r="29" spans="1:2" ht="15.6">
       <c r="A29" s="11" t="s">
@@ -2510,7 +2510,7 @@
   <dimension ref="A2:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A16" sqref="A16:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2526,20 +2526,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="38"/>
-      <c r="F2" s="32" t="s">
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="45"/>
+      <c r="F2" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="18" t="s">
@@ -2562,10 +2562,10 @@
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="40" t="s">
         <v>105</v>
       </c>
       <c r="C4" s="18" t="s">
@@ -2594,8 +2594,8 @@
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="33"/>
-      <c r="B5" s="33"/>
+      <c r="A5" s="40"/>
+      <c r="B5" s="40"/>
       <c r="C5" s="18" t="s">
         <v>120</v>
       </c>
@@ -2610,10 +2610,10 @@
       <c r="K5" s="20"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="41" t="s">
         <v>106</v>
       </c>
       <c r="C6" s="18" t="s">
@@ -2630,8 +2630,8 @@
       <c r="K6" s="20"/>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="35"/>
-      <c r="B7" s="35"/>
+      <c r="A7" s="42"/>
+      <c r="B7" s="42"/>
       <c r="C7" s="18" t="s">
         <v>125</v>
       </c>
@@ -2770,10 +2770,10 @@
       </c>
     </row>
     <row r="13" spans="1:12" s="21" customFormat="1">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="38" t="s">
         <v>138</v>
       </c>
       <c r="C13" s="20"/>
@@ -2782,17 +2782,17 @@
       </c>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="30"/>
-      <c r="B14" s="32"/>
+      <c r="A14" s="37"/>
+      <c r="B14" s="39"/>
       <c r="C14" s="19" t="s">
         <v>144</v>
       </c>
       <c r="D14" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="E14" s="39"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="19" t="s">
@@ -2804,9 +2804,9 @@
       <c r="D15" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
     </row>
     <row r="16" spans="1:12" ht="15.6">
       <c r="A16" s="22" t="s">
@@ -2815,9 +2815,9 @@
       <c r="B16" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="E16" s="40"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="39"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="26"/>
     </row>
     <row r="17" spans="1:7" ht="15.6">
       <c r="A17" s="19" t="s">
@@ -2826,9 +2826,9 @@
       <c r="B17" s="19" t="s">
         <v>155</v>
       </c>
-      <c r="E17" s="42"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="39"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="26"/>
     </row>
     <row r="18" spans="1:7" ht="15.6">
       <c r="A18" s="19" t="s">
@@ -2843,9 +2843,9 @@
       <c r="D18" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="E18" s="42"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="39"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="26"/>
     </row>
     <row r="19" spans="1:7" ht="15.6">
       <c r="A19" s="19" t="s">
@@ -2860,49 +2860,49 @@
       <c r="D19" s="19" t="s">
         <v>157</v>
       </c>
-      <c r="E19" s="44"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="39"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="26"/>
     </row>
     <row r="20" spans="1:7" ht="15.6">
-      <c r="E20" s="44"/>
-      <c r="F20" s="45"/>
-      <c r="G20" s="39"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="26"/>
     </row>
     <row r="21" spans="1:7" ht="15.6">
-      <c r="E21" s="44"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="39"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="26"/>
     </row>
     <row r="22" spans="1:7" ht="15.6">
-      <c r="E22" s="44"/>
-      <c r="F22" s="43"/>
-      <c r="G22" s="39"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="26"/>
     </row>
     <row r="23" spans="1:7" ht="15.6">
-      <c r="E23" s="44"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="39"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="26"/>
     </row>
     <row r="24" spans="1:7" ht="15.6">
-      <c r="E24" s="44"/>
-      <c r="F24" s="45"/>
-      <c r="G24" s="39"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="26"/>
     </row>
     <row r="25" spans="1:7" ht="15.6">
-      <c r="E25" s="44"/>
-      <c r="F25" s="41"/>
-      <c r="G25" s="39"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="26"/>
     </row>
     <row r="26" spans="1:7" ht="15.6">
-      <c r="E26" s="42"/>
-      <c r="F26" s="45"/>
-      <c r="G26" s="39"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="26"/>
     </row>
     <row r="27" spans="1:7">
-      <c r="E27" s="39"/>
-      <c r="F27" s="39"/>
-      <c r="G27" s="39"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
integracions de SRT y LDR con TBs
</commit_message>
<xml_diff>
--- a/archivos/comandos.xlsx
+++ b/archivos/comandos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emily\Desktop\CE4301-Proyecto1\archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89BF728A-390C-4AA5-B922-88FD6338C837}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9AC67C4-560B-4EF9-95F7-792F1BE3C1B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20520" yWindow="780" windowWidth="20640" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="720" yWindow="1548" windowWidth="12600" windowHeight="10128" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="166">
   <si>
     <t>Escritura y lectura *(tenemos que hablar de estos metodos)</t>
   </si>
@@ -377,9 +377,6 @@
     <t>ASM</t>
   </si>
   <si>
-    <t>OOOO11OOO1OOOOOOOOOOOO11OOOOOOOO</t>
-  </si>
-  <si>
     <t>mov R1,#3</t>
   </si>
   <si>
@@ -447,9 +444,6 @@
   </si>
   <si>
     <t>OO1OO1</t>
-  </si>
-  <si>
-    <t>str R1,#4</t>
   </si>
   <si>
     <r>
@@ -466,6 +460,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>oo1</t>
     </r>
@@ -477,9 +472,6 @@
     <t>STRMI</t>
   </si>
   <si>
-    <t>OO1OOOOOOOOOO1OOOOOOOOOOOOOOO1OO</t>
-  </si>
-  <si>
     <t>Destino</t>
   </si>
   <si>
@@ -529,6 +521,27 @@
   </si>
   <si>
     <t>OO11OOOOOOOOOOOOOOOOO1OOOOOOOOO</t>
+  </si>
+  <si>
+    <t>strmi R1</t>
+  </si>
+  <si>
+    <t>ldrmi R1</t>
+  </si>
+  <si>
+    <t>cada vez +4 en direccion</t>
+  </si>
+  <si>
+    <t>OO1OOOOOOOOO1O1OOOOOOOOOOOOOOOOO</t>
+  </si>
+  <si>
+    <t>OO1OO1OOO1O1OOOOOOOOOOOOOOOOOOOO</t>
+  </si>
+  <si>
+    <t>OO1O1OOOOOOO1OOOOOOOOOOOOOOOOOOO</t>
+  </si>
+  <si>
+    <t>OOOO11OOO1OOOOOOOOOOOOOOOOOOOO11</t>
   </si>
 </sst>
 </file>
@@ -545,39 +558,46 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -588,12 +608,14 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -608,7 +630,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -649,6 +671,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -751,7 +779,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -782,18 +810,6 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -805,18 +821,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -824,21 +858,24 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -852,6 +889,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2227,7 +2267,7 @@
   </sheetPr>
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
@@ -2254,7 +2294,7 @@
     </row>
     <row r="3" spans="1:6" ht="15.6">
       <c r="A3" s="7" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>37</v>
@@ -2271,7 +2311,7 @@
     </row>
     <row r="5" spans="1:6" ht="15.6">
       <c r="A5" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>40</v>
@@ -2331,12 +2371,12 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.6">
-      <c r="A13" s="23"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
+      <c r="A13" s="19"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
     </row>
     <row r="14" spans="1:6" ht="15.6">
       <c r="A14" s="12"/>
@@ -2487,8 +2527,8 @@
       </c>
     </row>
     <row r="34" spans="1:2" ht="14.4">
-      <c r="A34" s="24"/>
-      <c r="B34" s="24"/>
+      <c r="A34" s="20"/>
+      <c r="B34" s="20"/>
     </row>
     <row r="36" spans="1:2" ht="15.6">
       <c r="B36" s="17" t="s">
@@ -2507,407 +2547,410 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{935F8D7C-FEC4-4F7D-8C36-4AF6CEC33DFE}">
-  <dimension ref="A2:L27"/>
+  <dimension ref="A2:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:D16"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="11.296875" style="19" customWidth="1"/>
-    <col min="2" max="2" width="12.69921875" style="19" customWidth="1"/>
-    <col min="3" max="3" width="48.296875" style="19" customWidth="1"/>
-    <col min="4" max="5" width="14.69921875" style="19" customWidth="1"/>
-    <col min="6" max="6" width="10.8984375" style="19" customWidth="1"/>
-    <col min="7" max="11" width="8.796875" style="19"/>
-    <col min="12" max="13" width="16.69921875" style="19" customWidth="1"/>
-    <col min="14" max="16384" width="8.796875" style="19"/>
+    <col min="1" max="1" width="11.296875" style="25" customWidth="1"/>
+    <col min="2" max="2" width="12.69921875" style="25" customWidth="1"/>
+    <col min="3" max="3" width="48.296875" style="25" customWidth="1"/>
+    <col min="4" max="4" width="14.69921875" style="25" customWidth="1"/>
+    <col min="5" max="5" width="23.296875" style="25" customWidth="1"/>
+    <col min="6" max="6" width="10.8984375" style="25" customWidth="1"/>
+    <col min="7" max="11" width="8.796875" style="25"/>
+    <col min="12" max="13" width="16.69921875" style="25" customWidth="1"/>
+    <col min="14" max="16384" width="8.796875" style="25"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:12">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="44" t="s">
         <v>102</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="45"/>
-      <c r="F2" s="39" t="s">
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="46"/>
+      <c r="F2" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="25">
         <v>31</v>
       </c>
-      <c r="K3" s="19">
+      <c r="K3" s="25">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="39" t="s">
         <v>105</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="G4" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="H4" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="I4" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="J4" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="K4" s="26" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="38"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="D4" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="H4" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="I4" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="J4" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="K4" s="18" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="40"/>
-      <c r="B5" s="40"/>
-      <c r="C5" s="18" t="s">
+      <c r="D6" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="D5" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="41" t="s">
-        <v>107</v>
-      </c>
-      <c r="B6" s="41" t="s">
-        <v>106</v>
-      </c>
-      <c r="C6" s="18" t="s">
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="41"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D7" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="42"/>
-      <c r="B7" s="42"/>
-      <c r="C7" s="18" t="s">
+      <c r="F7" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="H7" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="I7" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="J7" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="K7" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="L7" s="25" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" s="47" t="s">
+        <v>165</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="H8" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="I8" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="J8" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="K8" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="L8" s="25" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="D7" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G7" s="22" t="s">
+      <c r="C9" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="F9" s="25">
+        <v>6</v>
+      </c>
+      <c r="G9" s="25">
+        <v>4</v>
+      </c>
+      <c r="H9" s="25">
+        <v>3</v>
+      </c>
+      <c r="I9" s="25">
+        <v>3</v>
+      </c>
+      <c r="J9" s="25">
+        <v>8</v>
+      </c>
+      <c r="K9" s="25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+    </row>
+    <row r="15" spans="1:12" ht="15.6">
+      <c r="A15" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="H7" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="I7" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="J7" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="K7" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="L7" s="19" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G8" s="22" t="s">
-        <v>141</v>
-      </c>
-      <c r="H8" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="I8" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="J8" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="K8" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="L8" s="19" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="F9" s="19">
-        <v>6</v>
-      </c>
-      <c r="G9" s="19">
-        <v>4</v>
-      </c>
-      <c r="H9" s="19">
-        <v>3</v>
-      </c>
-      <c r="I9" s="19">
-        <v>3</v>
-      </c>
-      <c r="J9" s="19">
-        <v>8</v>
-      </c>
-      <c r="K9" s="19">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>136</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" s="21" customFormat="1">
-      <c r="A13" s="36" t="s">
-        <v>142</v>
-      </c>
-      <c r="B13" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="37"/>
-      <c r="B14" s="39"/>
-      <c r="C14" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="19" t="s">
+      <c r="B15" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="E15" s="36" t="s">
+        <v>161</v>
+      </c>
+      <c r="F15" s="28"/>
+      <c r="G15" s="22"/>
+    </row>
+    <row r="16" spans="1:12" ht="15" customHeight="1">
+      <c r="A16" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="E16" s="36"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="22"/>
+    </row>
+    <row r="17" spans="1:7" ht="15.6">
+      <c r="A17" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="D17" s="25" t="s">
         <v>150</v>
       </c>
-      <c r="B15" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-    </row>
-    <row r="16" spans="1:12" ht="15.6">
-      <c r="A16" s="22" t="s">
-        <v>143</v>
-      </c>
-      <c r="B16" s="19" t="s">
+      <c r="E17" s="28"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="22"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.6">
+      <c r="A18" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="D18" s="25" t="s">
         <v>154</v>
       </c>
-      <c r="E16" s="27"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="26"/>
-    </row>
-    <row r="17" spans="1:7" ht="15.6">
-      <c r="A17" s="19" t="s">
-        <v>151</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>155</v>
-      </c>
-      <c r="E17" s="29"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="26"/>
-    </row>
-    <row r="18" spans="1:7" ht="15.6">
-      <c r="A18" s="19" t="s">
-        <v>152</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>156</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>161</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>153</v>
-      </c>
-      <c r="E18" s="29"/>
+      <c r="E18" s="31"/>
       <c r="F18" s="30"/>
-      <c r="G18" s="26"/>
+      <c r="G18" s="22"/>
     </row>
     <row r="19" spans="1:7" ht="15.6">
-      <c r="A19" s="19" t="s">
-        <v>158</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>159</v>
-      </c>
-      <c r="C19" s="19" t="s">
-        <v>160</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>157</v>
-      </c>
       <c r="E19" s="31"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="26"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="22"/>
     </row>
     <row r="20" spans="1:7" ht="15.6">
       <c r="E20" s="31"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="26"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="22"/>
     </row>
     <row r="21" spans="1:7" ht="15.6">
       <c r="E21" s="31"/>
       <c r="F21" s="30"/>
-      <c r="G21" s="26"/>
+      <c r="G21" s="22"/>
     </row>
     <row r="22" spans="1:7" ht="15.6">
       <c r="E22" s="31"/>
       <c r="F22" s="30"/>
-      <c r="G22" s="26"/>
+      <c r="G22" s="22"/>
     </row>
     <row r="23" spans="1:7" ht="15.6">
       <c r="E23" s="31"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="26"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="22"/>
     </row>
     <row r="24" spans="1:7" ht="15.6">
       <c r="E24" s="31"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="26"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="22"/>
     </row>
     <row r="25" spans="1:7" ht="15.6">
-      <c r="E25" s="31"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="26"/>
-    </row>
-    <row r="26" spans="1:7" ht="15.6">
-      <c r="E26" s="29"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="26"/>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="22"/>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
+  <mergeCells count="7">
+    <mergeCell ref="E15:E16"/>
     <mergeCell ref="F2:K2"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>

</xml_diff>

<commit_message>
Pruebas de operaciones completadas, faltan saltos
</commit_message>
<xml_diff>
--- a/archivos/comandos.xlsx
+++ b/archivos/comandos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emily\Desktop\CE4301-Proyecto1\archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9AC67C4-560B-4EF9-95F7-792F1BE3C1B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EDDA7FF-F9CD-4ABB-8D55-985D05C8F859}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="1548" windowWidth="12600" windowHeight="10128" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -851,6 +851,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -889,9 +892,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2279,10 +2279,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="34"/>
+      <c r="B1" s="35"/>
     </row>
     <row r="2" spans="1:6" ht="15.6">
       <c r="A2" s="7" t="s">
@@ -2383,10 +2383,10 @@
       <c r="B14" s="13"/>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="B15" s="34"/>
+      <c r="B15" s="35"/>
     </row>
     <row r="16" spans="1:6" ht="15.6">
       <c r="A16" s="7" t="s">
@@ -2481,10 +2481,10 @@
       <c r="B27" s="16"/>
     </row>
     <row r="28" spans="1:2" ht="15" customHeight="1">
-      <c r="A28" s="35" t="s">
+      <c r="A28" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="B28" s="34"/>
+      <c r="B28" s="35"/>
     </row>
     <row r="29" spans="1:2" ht="15.6">
       <c r="A29" s="11" t="s">
@@ -2550,7 +2550,7 @@
   <dimension ref="A2:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2567,20 +2567,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="45" t="s">
         <v>102</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="46"/>
-      <c r="F2" s="37" t="s">
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="47"/>
+      <c r="F2" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="26" t="s">
@@ -2603,10 +2603,10 @@
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="40" t="s">
         <v>105</v>
       </c>
       <c r="C4" s="26" t="s">
@@ -2635,8 +2635,8 @@
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="38"/>
-      <c r="B5" s="39"/>
+      <c r="A5" s="39"/>
+      <c r="B5" s="40"/>
       <c r="C5" s="26" t="s">
         <v>119</v>
       </c>
@@ -2651,10 +2651,10 @@
       <c r="K5" s="27"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="43" t="s">
         <v>106</v>
       </c>
       <c r="C6" s="26" t="s">
@@ -2671,8 +2671,8 @@
       <c r="K6" s="27"/>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="41"/>
-      <c r="B7" s="43"/>
+      <c r="A7" s="42"/>
+      <c r="B7" s="44"/>
       <c r="C7" s="26" t="s">
         <v>124</v>
       </c>
@@ -2708,7 +2708,7 @@
       <c r="B8" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="C8" s="47" t="s">
+      <c r="C8" s="33" t="s">
         <v>165</v>
       </c>
       <c r="D8" s="26" t="s">
@@ -2854,7 +2854,7 @@
       <c r="D15" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="E15" s="36" t="s">
+      <c r="E15" s="37" t="s">
         <v>161</v>
       </c>
       <c r="F15" s="28"/>
@@ -2873,7 +2873,7 @@
       <c r="D16" s="25" t="s">
         <v>160</v>
       </c>
-      <c r="E16" s="36"/>
+      <c r="E16" s="37"/>
       <c r="F16" s="30"/>
       <c r="G16" s="22"/>
     </row>

</xml_diff>